<commit_message>
labels and correspondind mails visible
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_ARJUN.xlsx
+++ b/Wave 5_React_Tracker_ARJUN.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>React Basics (Architecture, Concepts, Lifecycle)</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>24/08/2016</t>
+  </si>
+  <si>
+    <t>25/08/2016</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -407,7 +413,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -519,6 +525,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
completed all in reactJS assignment
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_ARJUN.xlsx
+++ b/Wave 5_React_Tracker_ARJUN.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>React Basics (Architecture, Concepts, Lifecycle)</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>27/08/2016</t>
+  </si>
+  <si>
+    <t>28/08/2016</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -427,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -561,6 +564,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>